<commit_message>
Ajout du diagramme du GANTT.
</commit_message>
<xml_diff>
--- a/Premier_Livrable/Document/Sae3_Matrice.xlsx
+++ b/Premier_Livrable/Document/Sae3_Matrice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j-lbz\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uvsq_22_23\sae3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169A353D-FF63-4808-8099-18E0C34B350C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1332003D-52AC-4C75-AFA9-8C4362019747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5364" yWindow="408" windowWidth="17280" windowHeight="8676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>Conception</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t xml:space="preserve">Nom de la tache </t>
+  </si>
+  <si>
+    <t>Jours --&gt;</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>Diagramme de GANTT</t>
+  </si>
+  <si>
+    <t>Matrice des antériorités</t>
   </si>
 </sst>
 </file>
@@ -207,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +262,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -263,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -277,6 +301,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,22 +643,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="67.88671875" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
@@ -646,8 +676,132 @@
       <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="14"/>
+      <c r="H1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <v>2</v>
+      </c>
+      <c r="K1">
+        <v>3</v>
+      </c>
+      <c r="L1">
+        <v>4</v>
+      </c>
+      <c r="M1">
+        <v>5</v>
+      </c>
+      <c r="N1">
+        <v>6</v>
+      </c>
+      <c r="O1">
+        <v>7</v>
+      </c>
+      <c r="P1">
+        <v>8</v>
+      </c>
+      <c r="Q1">
+        <v>9</v>
+      </c>
+      <c r="R1">
+        <v>11</v>
+      </c>
+      <c r="S1">
+        <v>12</v>
+      </c>
+      <c r="T1">
+        <v>13</v>
+      </c>
+      <c r="U1">
+        <v>14</v>
+      </c>
+      <c r="V1">
+        <v>15</v>
+      </c>
+      <c r="W1">
+        <v>16</v>
+      </c>
+      <c r="X1">
+        <v>17</v>
+      </c>
+      <c r="Y1">
+        <v>18</v>
+      </c>
+      <c r="Z1">
+        <v>19</v>
+      </c>
+      <c r="AA1">
+        <v>20</v>
+      </c>
+      <c r="AB1">
+        <v>21</v>
+      </c>
+      <c r="AC1">
+        <v>22</v>
+      </c>
+      <c r="AD1">
+        <v>23</v>
+      </c>
+      <c r="AE1">
+        <v>24</v>
+      </c>
+      <c r="AF1">
+        <v>25</v>
+      </c>
+      <c r="AG1">
+        <v>26</v>
+      </c>
+      <c r="AH1">
+        <v>27</v>
+      </c>
+      <c r="AI1">
+        <v>28</v>
+      </c>
+      <c r="AJ1">
+        <v>29</v>
+      </c>
+      <c r="AK1">
+        <v>30</v>
+      </c>
+      <c r="AL1">
+        <v>31</v>
+      </c>
+      <c r="AM1">
+        <v>32</v>
+      </c>
+      <c r="AN1">
+        <v>33</v>
+      </c>
+      <c r="AO1">
+        <v>34</v>
+      </c>
+      <c r="AP1">
+        <v>35</v>
+      </c>
+      <c r="AQ1">
+        <v>36</v>
+      </c>
+      <c r="AR1">
+        <v>37</v>
+      </c>
+      <c r="AS1">
+        <v>38</v>
+      </c>
+      <c r="AT1">
+        <v>39</v>
+      </c>
+      <c r="AU1">
+        <v>40</v>
+      </c>
+      <c r="AV1" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -666,8 +820,15 @@
       <c r="F2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="14"/>
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="AV2" s="14"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>15</v>
@@ -684,8 +845,20 @@
       <c r="F3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="14"/>
+      <c r="H3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="AV3" s="14"/>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -702,8 +875,15 @@
       <c r="F4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="14"/>
+      <c r="H4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="AV4" s="14"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -720,8 +900,17 @@
       <c r="F5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="14"/>
+      <c r="H5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="AV5" s="14"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
         <v>48</v>
@@ -738,8 +927,15 @@
       <c r="F6" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="14"/>
+      <c r="H6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="AV6" s="14"/>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -756,8 +952,14 @@
       <c r="F7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="14"/>
+      <c r="H7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="AV7" s="14"/>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
         <v>26</v>
@@ -774,11 +976,20 @@
       <c r="F8" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="14"/>
+      <c r="H8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="AV8" s="14"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="14"/>
+      <c r="AV9" s="14"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -797,8 +1008,14 @@
       <c r="F10" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="14"/>
+      <c r="H10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z10" s="5"/>
+      <c r="AV10" s="14"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
         <v>18</v>
@@ -815,11 +1032,20 @@
       <c r="F11" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="14"/>
+      <c r="H11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AV11" s="14"/>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="14"/>
+      <c r="AV12" s="14"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
@@ -838,8 +1064,17 @@
       <c r="F13" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="14"/>
+      <c r="H13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AV13" s="14"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="7" t="s">
         <v>10</v>
@@ -856,11 +1091,21 @@
       <c r="F14" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="14"/>
+      <c r="H14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AV14" s="14"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="14"/>
+      <c r="AV15" s="14"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
@@ -879,8 +1124,18 @@
       <c r="F16" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="14"/>
+      <c r="H16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
+      <c r="AV16" s="14"/>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
         <v>11</v>
@@ -897,8 +1152,18 @@
       <c r="F17" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="14"/>
+      <c r="H17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
+      <c r="AV17" s="14"/>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>12</v>
@@ -915,8 +1180,18 @@
       <c r="F18" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="14"/>
+      <c r="H18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="9"/>
+      <c r="AV18" s="14"/>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
         <v>13</v>
@@ -933,8 +1208,16 @@
       <c r="F19" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="14"/>
+      <c r="H19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AV19" s="14"/>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
         <v>14</v>
@@ -951,11 +1234,20 @@
       <c r="F20" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="14"/>
+      <c r="H20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AV20" s="14"/>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="14"/>
+      <c r="AV21" s="14"/>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>24</v>
       </c>
@@ -974,8 +1266,18 @@
       <c r="F22" s="11">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="14"/>
+      <c r="H22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL22" s="11"/>
+      <c r="AM22" s="11"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="11"/>
+      <c r="AP22" s="11"/>
+      <c r="AV22" s="14"/>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>21</v>
@@ -992,8 +1294,16 @@
       <c r="F23" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="14"/>
+      <c r="H23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="11"/>
+      <c r="AS23" s="11"/>
+      <c r="AV23" s="14"/>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>22</v>
@@ -1009,6 +1319,21 @@
       </c>
       <c r="F24" s="11">
         <v>11</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT24" s="11"/>
+      <c r="AU24" s="11"/>
+      <c r="AV24" s="14"/>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>